<commit_message>
A simulation engine independent of PySD, not using swap python file.
</commit_message>
<xml_diff>
--- a/supportive_files/basic_behaviors.xlsx
+++ b/supportive_files/basic_behaviors.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonker/OneDrive/SFD_Canvas/Stock_and_Flow_Canvas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonker/OneDrive/SFD_Canvas/Stock_and_Flow_Canvas/supportive_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{E9F23EB0-66AC-034C-9610-7B95F73F4C42}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{02434C4E-C221-6241-8E2D-44054FA65D82}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{E9F23EB0-66AC-034C-9610-7B95F73F4C42}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{122FF0A7-F0C0-EC41-A1B4-6C246FDECB3C}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16900" xr2:uid="{2D83422D-6A31-2444-AEF0-6678B38B77BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4C7BD0-24E7-604E-B5A1-8BA59114F1DD}">
-  <dimension ref="A1:Y102"/>
+  <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,7 +467,7 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +544,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -570,7 +570,7 @@
         <v>100</v>
       </c>
       <c r="I2">
-        <v>-1</v>
+        <v>99</v>
       </c>
       <c r="J2">
         <v>100</v>
@@ -620,8 +620,12 @@
       <c r="Y2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z2">
+        <f>I2+100</f>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.25</v>
       </c>
@@ -647,7 +651,7 @@
         <v>99</v>
       </c>
       <c r="I3">
-        <v>-1.0462499999999999</v>
+        <v>98.953749999999999</v>
       </c>
       <c r="J3">
         <v>95.05</v>
@@ -697,8 +701,12 @@
       <c r="Y3">
         <v>1.096525</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z66" si="0">I3+100</f>
+        <v>198.95375000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.5</v>
       </c>
@@ -724,7 +732,7 @@
         <v>98</v>
       </c>
       <c r="I4">
-        <v>-1.0946390625</v>
+        <v>98.905360937500006</v>
       </c>
       <c r="J4">
         <v>90.347499999999997</v>
@@ -774,8 +782,12 @@
       <c r="Y4">
         <v>1.2022638796</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>198.90536093750001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.75</v>
       </c>
@@ -801,7 +813,7 @@
         <v>97</v>
       </c>
       <c r="I5">
-        <v>-1.14526611914</v>
+        <v>98.854733880859996</v>
       </c>
       <c r="J5">
         <v>85.880125000000007</v>
@@ -851,8 +863,12 @@
       <c r="Y5">
         <v>1.3180753053900001</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>198.85473388086001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -878,7 +894,7 @@
         <v>96</v>
       </c>
       <c r="I6">
-        <v>-1.1982346771500001</v>
+        <v>98.801765322850002</v>
       </c>
       <c r="J6">
         <v>81.636118749999994</v>
@@ -928,8 +944,12 @@
       <c r="Y6">
         <v>1.4448937582100001</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>198.80176532285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.25</v>
       </c>
@@ -955,7 +975,7 @@
         <v>95</v>
       </c>
       <c r="I7">
-        <v>-1.25365303097</v>
+        <v>98.74634696903</v>
       </c>
       <c r="J7">
         <v>77.604312812499998</v>
@@ -1005,8 +1025,12 @@
       <c r="Y7">
         <v>1.58373537462</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z7">
+        <f t="shared" si="0"/>
+        <v>198.74634696903001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1.5</v>
       </c>
@@ -1032,7 +1056,7 @@
         <v>94</v>
       </c>
       <c r="I8">
-        <v>-1.31163448365</v>
+        <v>98.688365516350004</v>
       </c>
       <c r="J8">
         <v>73.774097171899996</v>
@@ -1082,8 +1106,12 @@
       <c r="Y8">
         <v>1.7357040613500001</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z8">
+        <f t="shared" si="0"/>
+        <v>198.68836551635002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1.75</v>
       </c>
@@ -1109,7 +1137,7 @@
         <v>93</v>
       </c>
       <c r="I9">
-        <v>-1.37229757852</v>
+        <v>98.627702421479995</v>
       </c>
       <c r="J9">
         <v>70.135392313300002</v>
@@ -1159,8 +1187,12 @@
       <c r="Y9">
         <v>1.9019978554600001</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z9">
+        <f t="shared" si="0"/>
+        <v>198.62770242148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1186,7 +1218,7 @@
         <v>92</v>
       </c>
       <c r="I10">
-        <v>-1.4357663415299999</v>
+        <v>98.564233658470002</v>
       </c>
       <c r="J10">
         <v>66.678622697600005</v>
@@ -1236,8 +1268,12 @@
       <c r="Y10">
         <v>2.0839154904199999</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z10">
+        <f t="shared" si="0"/>
+        <v>198.56423365847002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2.25</v>
       </c>
@@ -1263,7 +1299,7 @@
         <v>91</v>
       </c>
       <c r="I11">
-        <v>-1.5021705348200001</v>
+        <v>98.497829465180004</v>
       </c>
       <c r="J11">
         <v>63.394691562699997</v>
@@ -1313,8 +1349,12 @@
       <c r="Y11">
         <v>2.28286311456</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z11">
+        <f t="shared" si="0"/>
+        <v>198.49782946518002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2.5</v>
       </c>
@@ -1340,7 +1380,7 @@
         <v>90</v>
       </c>
       <c r="I12">
-        <v>-1.5716459220600001</v>
+        <v>98.42835407794</v>
       </c>
       <c r="J12">
         <v>60.274956984600003</v>
@@ -1390,8 +1430,12 @@
       <c r="Y12">
         <v>2.5003610908299998</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z12">
+        <f t="shared" si="0"/>
+        <v>198.42835407794001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2.75</v>
       </c>
@@ -1417,7 +1461,7 @@
         <v>89</v>
       </c>
       <c r="I13">
-        <v>-1.6443345459500001</v>
+        <v>98.355665454049998</v>
       </c>
       <c r="J13">
         <v>57.311209135399999</v>
@@ -1467,8 +1511,12 @@
       <c r="Y13">
         <v>2.7380507867400001</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z13">
+        <f t="shared" si="0"/>
+        <v>198.35566545404998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1494,7 +1542,7 @@
         <v>88</v>
       </c>
       <c r="I14">
-        <v>-1.7203850187</v>
+        <v>98.2796149813</v>
       </c>
       <c r="J14">
         <v>54.495648678599999</v>
@@ -1544,8 +1592,12 @@
       <c r="Y14">
         <v>2.99770123939</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z14">
+        <f t="shared" si="0"/>
+        <v>198.2796149813</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3.25</v>
       </c>
@@ -1571,7 +1623,7 @@
         <v>87</v>
       </c>
       <c r="I15">
-        <v>-1.7999528258199999</v>
+        <v>98.20004717418</v>
       </c>
       <c r="J15">
         <v>51.820866244699999</v>
@@ -1621,8 +1673,12 @@
       <c r="Y15">
         <v>3.28121555282</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z15">
+        <f t="shared" si="0"/>
+        <v>198.20004717417999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3.5</v>
       </c>
@@ -1648,7 +1704,7 @@
         <v>86</v>
       </c>
       <c r="I16">
-        <v>-1.88320064401</v>
+        <v>98.116799355989997</v>
       </c>
       <c r="J16">
         <v>49.279822932400002</v>
@@ -1698,8 +1754,12 @@
       <c r="Y16">
         <v>3.5906368531099999</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z16">
+        <f t="shared" si="0"/>
+        <v>198.11679935599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3.75</v>
       </c>
@@ -1725,7 +1785,7 @@
         <v>85</v>
       </c>
       <c r="I17">
-        <v>-1.9702986737999999</v>
+        <v>98.029701326199998</v>
       </c>
       <c r="J17">
         <v>46.865831785799998</v>
@@ -1775,8 +1835,12 @@
       <c r="Y17">
         <v>3.9281535901</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z17">
+        <f t="shared" si="0"/>
+        <v>198.02970132619998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1802,7 +1866,7 @@
         <v>84</v>
       </c>
       <c r="I18">
-        <v>-2.0614249874600001</v>
+        <v>97.938575012539999</v>
       </c>
       <c r="J18">
         <v>44.5725401965</v>
@@ -1852,8 +1916,12 @@
       <c r="Y18">
         <v>4.2961039342699996</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z18">
+        <f t="shared" si="0"/>
+        <v>197.93857501254001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4.25</v>
       </c>
@@ -1879,7 +1947,7 @@
         <v>83</v>
       </c>
       <c r="I19">
-        <v>-2.1567658931299998</v>
+        <v>97.84323410687</v>
       </c>
       <c r="J19">
         <v>42.393913186699997</v>
@@ -1929,8 +1997,12 @@
       <c r="Y19">
         <v>4.6969789715700001</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z19">
+        <f t="shared" si="0"/>
+        <v>197.84323410687</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4.5</v>
       </c>
@@ -1956,7 +2028,7 @@
         <v>82</v>
       </c>
       <c r="I20">
-        <v>-2.2565163156899999</v>
+        <v>97.743483684310007</v>
       </c>
       <c r="J20">
         <v>40.324217527400002</v>
@@ -2006,8 +2078,12 @@
       <c r="Y20">
         <v>5.1334243501300003</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z20">
+        <f t="shared" si="0"/>
+        <v>197.74348368431001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4.75</v>
       </c>
@@ -2033,7 +2109,7 @@
         <v>81</v>
       </c>
       <c r="I21">
-        <v>-2.36088019529</v>
+        <v>97.639119804710006</v>
       </c>
       <c r="J21">
         <v>38.358006650999997</v>
@@ -2083,8 +2159,12 @@
       <c r="Y21">
         <v>5.6082399798499996</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z21">
+        <f t="shared" si="0"/>
+        <v>197.63911980470999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2110,7 +2190,7 @@
         <v>80</v>
       </c>
       <c r="I22">
-        <v>-2.47007090432</v>
+        <v>97.529929095680004</v>
       </c>
       <c r="J22">
         <v>36.490106318400002</v>
@@ -2160,8 +2240,12 @@
       <c r="Y22">
         <v>6.1243773310999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z22">
+        <f t="shared" si="0"/>
+        <v>197.52992909568002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5.25</v>
       </c>
@@ -2187,7 +2271,7 @@
         <v>79</v>
       </c>
       <c r="I23">
-        <v>-2.5843116836500002</v>
+        <v>97.41568831635</v>
       </c>
       <c r="J23">
         <v>34.715601002500001</v>
@@ -2237,8 +2321,12 @@
       <c r="Y23">
         <v>6.6849338231299997</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z23">
+        <f t="shared" si="0"/>
+        <v>197.41568831634999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5.5</v>
       </c>
@@ -2264,7 +2352,7 @@
         <v>78</v>
       </c>
       <c r="I24">
-        <v>-2.7038360990200001</v>
+        <v>97.296163900980005</v>
       </c>
       <c r="J24">
         <v>33.029820952400001</v>
@@ -2314,8 +2402,12 @@
       <c r="Y24">
         <v>7.2931437391799996</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z24">
+        <f t="shared" si="0"/>
+        <v>197.29616390097999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5.75</v>
       </c>
@@ -2341,7 +2433,7 @@
         <v>77</v>
       </c>
       <c r="I25">
-        <v>-2.8288885185899999</v>
+        <v>97.171111481409994</v>
       </c>
       <c r="J25">
         <v>31.428329904800002</v>
@@ -2391,8 +2483,12 @@
       <c r="Y25">
         <v>7.9523650567899997</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z25">
+        <f t="shared" si="0"/>
+        <v>197.17111148140998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>6</v>
       </c>
@@ -2418,7 +2514,7 @@
         <v>76</v>
       </c>
       <c r="I26">
-        <v>-2.9597246125800001</v>
+        <v>97.040275387419996</v>
       </c>
       <c r="J26">
         <v>29.9069134095</v>
@@ -2468,8 +2564,12 @@
       <c r="Y26">
         <v>8.6660615425799996</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z26">
+        <f t="shared" si="0"/>
+        <v>197.04027538742</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>6.25</v>
       </c>
@@ -2495,7 +2595,7 @@
         <v>75</v>
       </c>
       <c r="I27">
-        <v>-3.0966118759099999</v>
+        <v>96.90338812409</v>
       </c>
       <c r="J27">
         <v>28.461567739100001</v>
@@ -2545,8 +2645,12 @@
       <c r="Y27">
         <v>9.4377794358799996</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z27">
+        <f t="shared" si="0"/>
+        <v>196.90338812408999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>6.5</v>
       </c>
@@ -2572,7 +2676,7 @@
         <v>74</v>
       </c>
       <c r="I28">
-        <v>-3.2398301751699998</v>
+        <v>96.760169824830001</v>
       </c>
       <c r="J28">
         <v>27.088489352100002</v>
@@ -2622,8 +2726,12 @@
       <c r="Y28">
         <v>10.271118042199999</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z28">
+        <f t="shared" si="0"/>
+        <v>196.76016982483</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>6.75</v>
       </c>
@@ -2649,7 +2757,7 @@
         <v>73</v>
       </c>
       <c r="I29">
-        <v>-3.3896723207699999</v>
+        <v>96.610327679229997</v>
       </c>
       <c r="J29">
         <v>25.784064884500001</v>
@@ -2699,8 +2807,12 @@
       <c r="Y29">
         <v>11.169693582100001</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z29">
+        <f t="shared" si="0"/>
+        <v>196.61032767923001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>7</v>
       </c>
@@ -2726,7 +2838,7 @@
         <v>72</v>
       </c>
       <c r="I30">
-        <v>-3.5464446656100002</v>
+        <v>96.453555334390003</v>
       </c>
       <c r="J30">
         <v>24.544861640299999</v>
@@ -2776,8 +2888,12 @@
       <c r="Y30">
         <v>12.1370957031</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z30">
+        <f t="shared" si="0"/>
+        <v>196.45355533438999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>7.25</v>
       </c>
@@ -2803,7 +2919,7 @@
         <v>71</v>
       </c>
       <c r="I31">
-        <v>-3.7104677313900001</v>
+        <v>96.289532268610003</v>
       </c>
       <c r="J31">
         <v>23.367618558299998</v>
@@ -2853,8 +2969,12 @@
       <c r="Y31">
         <v>13.1768361693</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z31">
+        <f t="shared" si="0"/>
+        <v>196.28953226861</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>7.5</v>
       </c>
@@ -2880,7 +3000,7 @@
         <v>70</v>
       </c>
       <c r="I32">
-        <v>-3.8820768639700001</v>
+        <v>96.117923136030001</v>
       </c>
       <c r="J32">
         <v>22.2492376304</v>
@@ -2930,8 +3050,12 @@
       <c r="Y32">
         <v>14.2922894097</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z32">
+        <f t="shared" si="0"/>
+        <v>196.11792313603002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>7.75</v>
       </c>
@@ -2957,7 +3081,7 @@
         <v>69</v>
       </c>
       <c r="I33">
-        <v>-4.0616229189300004</v>
+        <v>95.938377081070001</v>
       </c>
       <c r="J33">
         <v>21.186775748799999</v>
@@ -3007,8 +3131,12 @@
       <c r="Y33">
         <v>15.4866248289</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z33">
+        <f t="shared" si="0"/>
+        <v>195.93837708107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8</v>
       </c>
@@ -3034,7 +3162,7 @@
         <v>68</v>
       </c>
       <c r="I34">
-        <v>-4.2494729789300001</v>
+        <v>95.750527021069999</v>
       </c>
       <c r="J34">
         <v>20.177436961400002</v>
@@ -3084,8 +3212,12 @@
       <c r="Y34">
         <v>16.762731089900001</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z34">
+        <f t="shared" si="0"/>
+        <v>195.75052702107001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8.25</v>
       </c>
@@ -3111,7 +3243,7 @@
         <v>67</v>
       </c>
       <c r="I35">
-        <v>-4.4460111042100001</v>
+        <v>95.553988895789999</v>
       </c>
       <c r="J35">
         <v>19.218565113299999</v>
@@ -3161,8 +3293,12 @@
       <c r="Y35">
         <v>18.123132946399998</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z35">
+        <f t="shared" si="0"/>
+        <v>195.55398889578998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>8.5</v>
       </c>
@@ -3188,7 +3324,7 @@
         <v>66</v>
       </c>
       <c r="I36">
-        <v>-4.6516391177800003</v>
+        <v>95.348360882219993</v>
       </c>
       <c r="J36">
         <v>18.3076368577</v>
@@ -3238,8 +3374,12 @@
       <c r="Y36">
         <v>19.569901659599999</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z36">
+        <f t="shared" si="0"/>
+        <v>195.34836088221999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>8.75</v>
       </c>
@@ -3265,7 +3405,7 @@
         <v>65</v>
       </c>
       <c r="I37">
-        <v>-4.8667774269699997</v>
+        <v>95.133222573029997</v>
       </c>
       <c r="J37">
         <v>17.442255014800001</v>
@@ -3315,8 +3455,12 @@
       <c r="Y37">
         <v>21.1045605467</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z37">
+        <f t="shared" si="0"/>
+        <v>195.13322257303</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>9</v>
       </c>
@@ -3342,7 +3486,7 @@
         <v>64</v>
       </c>
       <c r="I38">
-        <v>-5.0918658829699996</v>
+        <v>94.908134117030002</v>
       </c>
       <c r="J38">
         <v>16.620142263999998</v>
@@ -3392,8 +3536,12 @@
       <c r="Y38">
         <v>22.727987786</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z38">
+        <f t="shared" si="0"/>
+        <v>194.90813411702999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>9.25</v>
       </c>
@@ -3419,7 +3567,7 @@
         <v>63</v>
       </c>
       <c r="I39">
-        <v>-5.3273646800599996</v>
+        <v>94.672635319939999</v>
       </c>
       <c r="J39">
         <v>15.839135150800001</v>
@@ -3469,8 +3617,12 @@
       <c r="Y39">
         <v>24.4403192021</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z39">
+        <f t="shared" si="0"/>
+        <v>194.67263531994001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>9.5</v>
       </c>
@@ -3496,7 +3648,7 @@
         <v>62</v>
       </c>
       <c r="I40">
-        <v>-5.5737552965099999</v>
+        <v>94.426244703489999</v>
       </c>
       <c r="J40">
         <v>15.0971783933</v>
@@ -3546,8 +3698,12 @@
       <c r="Y40">
         <v>26.240854351599999</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z40">
+        <f t="shared" si="0"/>
+        <v>194.42624470349</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>9.75</v>
       </c>
@@ -3573,7 +3729,7 @@
         <v>61</v>
       </c>
       <c r="I41">
-        <v>-5.8315414789700002</v>
+        <v>94.168458521030004</v>
       </c>
       <c r="J41">
         <v>14.392319473600001</v>
@@ -3623,8 +3779,12 @@
       <c r="Y41">
         <v>28.1279697748</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z41">
+        <f t="shared" si="0"/>
+        <v>194.16845852103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>10</v>
       </c>
@@ -3650,7 +3810,7 @@
         <v>60</v>
       </c>
       <c r="I42">
-        <v>-6.1012502723799997</v>
+        <v>93.89874972762</v>
       </c>
       <c r="J42">
         <v>13.7227034999</v>
@@ -3700,8 +3860,12 @@
       <c r="Y42">
         <v>30.0990437112</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z42">
+        <f t="shared" si="0"/>
+        <v>193.89874972761999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>10.25</v>
       </c>
@@ -3727,7 +3891,7 @@
         <v>59</v>
       </c>
       <c r="I43">
-        <v>-6.3834330974700002</v>
+        <v>93.616566902529996</v>
       </c>
       <c r="J43">
         <v>13.0865683249</v>
@@ -3777,8 +3941,12 @@
       <c r="Y43">
         <v>32.1503968516</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z43">
+        <f t="shared" si="0"/>
+        <v>193.61656690253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>10.5</v>
       </c>
@@ -3804,7 +3972,7 @@
         <v>58</v>
       </c>
       <c r="I44">
-        <v>-6.6786668782299996</v>
+        <v>93.321333121769996</v>
       </c>
       <c r="J44">
         <v>12.4822399087</v>
@@ -3854,8 +4022,12 @@
       <c r="Y44">
         <v>34.2772537273</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z44">
+        <f t="shared" si="0"/>
+        <v>193.32133312177001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>10.75</v>
       </c>
@@ -3881,7 +4053,7 @@
         <v>57</v>
       </c>
       <c r="I45">
-        <v>-6.9875552213500001</v>
+        <v>93.012444778650007</v>
       </c>
       <c r="J45">
         <v>11.9081279133</v>
@@ -3931,8 +4103,12 @@
       <c r="Y45">
         <v>36.473729095700001</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z45">
+        <f t="shared" si="0"/>
+        <v>193.01244477865001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>11</v>
       </c>
@@ -3958,7 +4134,7 @@
         <v>56</v>
       </c>
       <c r="I46">
-        <v>-7.3107296503399999</v>
+        <v>92.689270349660006</v>
       </c>
       <c r="J46">
         <v>11.362721517600001</v>
@@ -4008,8 +4184,12 @@
       <c r="Y46">
         <v>38.732843091299998</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z46">
+        <f t="shared" si="0"/>
+        <v>192.68927034966001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>11.25</v>
       </c>
@@ -4035,7 +4215,7 @@
         <v>55</v>
       </c>
       <c r="I47">
-        <v>-7.64885089667</v>
+        <v>92.351149103330002</v>
       </c>
       <c r="J47">
         <v>10.8445854417</v>
@@ -4085,8 +4265,12 @@
       <c r="Y47">
         <v>41.046567987099998</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z47">
+        <f t="shared" si="0"/>
+        <v>192.35114910332999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>11.5</v>
       </c>
@@ -4112,7 +4296,7 @@
         <v>54</v>
       </c>
       <c r="I48">
-        <v>-8.0026102506400001</v>
+        <v>91.997389749359996</v>
       </c>
       <c r="J48">
         <v>10.3523561696</v>
@@ -4162,8 +4346,12 @@
       <c r="Y48">
         <v>43.405908140900003</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z48">
+        <f t="shared" si="0"/>
+        <v>191.99738974936</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>11.75</v>
       </c>
@@ -4189,7 +4377,7 @@
         <v>53</v>
       </c>
       <c r="I49">
-        <v>-8.3727309747300005</v>
+        <v>91.627269025269996</v>
       </c>
       <c r="J49">
         <v>9.8847383611499993</v>
@@ -4239,8 +4427,12 @@
       <c r="Y49">
         <v>45.801013144599999</v>
       </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z49">
+        <f t="shared" si="0"/>
+        <v>191.62726902526998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>12</v>
       </c>
@@ -4266,7 +4458,7 @@
         <v>52</v>
       </c>
       <c r="I50">
-        <v>-8.7599697823099998</v>
+        <v>91.240030217690006</v>
       </c>
       <c r="J50">
         <v>9.4405014431000005</v>
@@ -4316,8 +4508,12 @@
       <c r="Y50">
         <v>48.221322441300003</v>
       </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z50">
+        <f t="shared" si="0"/>
+        <v>191.24003021768999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>12.25</v>
       </c>
@@ -4343,7 +4539,7 @@
         <v>51</v>
       </c>
       <c r="I51">
-        <v>-9.1651183847399995</v>
+        <v>90.834881615260002</v>
       </c>
       <c r="J51">
         <v>9.0184763709400002</v>
@@ -4393,8 +4589,12 @@
       <c r="Y51">
         <v>50.655737839799997</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z51">
+        <f t="shared" si="0"/>
+        <v>190.83488161526</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>12.5</v>
       </c>
@@ -4420,7 +4620,7 @@
         <v>50</v>
       </c>
       <c r="I52">
-        <v>-9.5890051100400004</v>
+        <v>90.410994889959994</v>
       </c>
       <c r="J52">
         <v>8.6175525523900003</v>
@@ -4470,8 +4670,12 @@
       <c r="Y52">
         <v>53.092818597499999</v>
       </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z52">
+        <f t="shared" si="0"/>
+        <v>190.41099488995999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>12.75</v>
       </c>
@@ -4497,7 +4701,7 @@
         <v>49</v>
       </c>
       <c r="I53">
-        <v>-10.0324965964</v>
+        <v>89.967503403600006</v>
       </c>
       <c r="J53">
         <v>8.23667492477</v>
@@ -4547,8 +4751,12 @@
       <c r="Y53">
         <v>55.520992208700001</v>
       </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z53">
+        <f t="shared" si="0"/>
+        <v>189.96750340360001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>13</v>
       </c>
@@ -4574,7 +4782,7 @@
         <v>48</v>
       </c>
       <c r="I54">
-        <v>-10.496499564000001</v>
+        <v>89.503500435999996</v>
       </c>
       <c r="J54">
         <v>7.8748411785399997</v>
@@ -4624,8 +4832,12 @@
       <c r="Y54">
         <v>57.928772887699999</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z54">
+        <f t="shared" si="0"/>
+        <v>189.503500436</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>13.25</v>
       </c>
@@ -4651,7 +4863,7 @@
         <v>47</v>
       </c>
       <c r="I55">
-        <v>-10.9819626688</v>
+        <v>89.018037331200006</v>
       </c>
       <c r="J55">
         <v>7.5310991196100003</v>
@@ -4701,8 +4913,12 @@
       <c r="Y55">
         <v>60.304979084099998</v>
       </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z55">
+        <f t="shared" si="0"/>
+        <v>189.01803733119999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>13.5</v>
       </c>
@@ -4728,7 +4944,7 @@
         <v>46</v>
       </c>
       <c r="I56">
-        <v>-11.4898784422</v>
+        <v>88.510121557800005</v>
       </c>
       <c r="J56">
         <v>7.2045441636299996</v>
@@ -4778,8 +4994,12 @@
       <c r="Y56">
         <v>62.638941305099998</v>
       </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z56">
+        <f t="shared" si="0"/>
+        <v>188.51012155780001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>13.75</v>
       </c>
@@ -4805,7 +5025,7 @@
         <v>45</v>
       </c>
       <c r="I57">
-        <v>-12.021285320200001</v>
+        <v>87.978714679799992</v>
       </c>
       <c r="J57">
         <v>6.8943169554499999</v>
@@ -4855,8 +5075,12 @@
       <c r="Y57">
         <v>64.920692038699997</v>
       </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z57">
+        <f t="shared" si="0"/>
+        <v>187.97871467979999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>14</v>
       </c>
@@ -4882,7 +5106,7 @@
         <v>44</v>
       </c>
       <c r="I58">
-        <v>-12.577269766200001</v>
+        <v>87.422730233799996</v>
       </c>
       <c r="J58">
         <v>6.5996011076799999</v>
@@ -4932,8 +5156,12 @@
       <c r="Y58">
         <v>67.141130664000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z58">
+        <f t="shared" si="0"/>
+        <v>187.4227302338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>14.25</v>
       </c>
@@ -4959,7 +5187,7 @@
         <v>43</v>
       </c>
       <c r="I59">
-        <v>-13.1589684929</v>
+        <v>86.841031507099999</v>
       </c>
       <c r="J59">
         <v>6.3196210522899996</v>
@@ -5009,8 +5237,12 @@
       <c r="Y59">
         <v>69.292157762599999</v>
       </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z59">
+        <f t="shared" si="0"/>
+        <v>186.84103150710001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>14.5</v>
       </c>
@@ -5036,7 +5268,7 @@
         <v>42</v>
       </c>
       <c r="I60">
-        <v>-13.7675707857</v>
+        <v>86.232429214299998</v>
       </c>
       <c r="J60">
         <v>6.0536399996799997</v>
@@ -5086,8 +5318,12 @@
       <c r="Y60">
         <v>71.3667750953</v>
       </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z60">
+        <f t="shared" si="0"/>
+        <v>186.2324292143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>14.75</v>
       </c>
@@ -5113,7 +5349,7 @@
         <v>41</v>
       </c>
       <c r="I61">
-        <v>-14.404320934599999</v>
+        <v>85.595679065400006</v>
       </c>
       <c r="J61">
         <v>5.8009579996899996</v>
@@ -5163,8 +5399,12 @@
       <c r="Y61">
         <v>73.359149494199997</v>
       </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z61">
+        <f t="shared" si="0"/>
+        <v>185.59567906540002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>15</v>
       </c>
@@ -5190,7 +5430,7 @@
         <v>40</v>
       </c>
       <c r="I62">
-        <v>-15.070520777800001</v>
+        <v>84.929479222200001</v>
       </c>
       <c r="J62">
         <v>5.5609100997100001</v>
@@ -5240,8 +5480,12 @@
       <c r="Y62">
         <v>75.264640875799998</v>
       </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z62">
+        <f t="shared" si="0"/>
+        <v>184.9294792222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>15.25</v>
       </c>
@@ -5267,7 +5511,7 @@
         <v>39</v>
       </c>
       <c r="I63">
-        <v>-15.767532363799999</v>
+        <v>84.232467636199999</v>
       </c>
       <c r="J63">
         <v>5.3328645947200002</v>
@@ -5317,8 +5561,12 @@
       <c r="Y63">
         <v>77.079796349099993</v>
       </c>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z63">
+        <f t="shared" si="0"/>
+        <v>184.2324676362</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>15.5</v>
       </c>
@@ -5344,7 +5592,7 @@
         <v>38</v>
       </c>
       <c r="I64">
-        <v>-16.496780735600002</v>
+        <v>83.503219264400002</v>
       </c>
       <c r="J64">
         <v>5.1162213649900004</v>
@@ -5394,8 +5642,12 @@
       <c r="Y64">
         <v>78.802313863099997</v>
       </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z64">
+        <f t="shared" si="0"/>
+        <v>183.5032192644</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>15.75</v>
       </c>
@@ -5421,7 +5673,7 @@
         <v>37</v>
       </c>
       <c r="I65">
-        <v>-17.259756844599998</v>
+        <v>82.740243155400009</v>
       </c>
       <c r="J65">
         <v>4.9104102967400003</v>
@@ -5471,8 +5723,12 @@
       <c r="Y65">
         <v>80.4309799113</v>
       </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z65">
+        <f t="shared" si="0"/>
+        <v>182.74024315540001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>16</v>
       </c>
@@ -5498,7 +5754,7 @@
         <v>36</v>
       </c>
       <c r="I66">
-        <v>-18.058020598700001</v>
+        <v>81.941979401300003</v>
       </c>
       <c r="J66">
         <v>4.7148897819000002</v>
@@ -5548,8 +5804,12 @@
       <c r="Y66">
         <v>81.965586486399999</v>
       </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z66">
+        <f t="shared" si="0"/>
+        <v>181.94197940129999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>16.25</v>
       </c>
@@ -5575,7 +5835,7 @@
         <v>35</v>
       </c>
       <c r="I67">
-        <v>-18.8932040513</v>
+        <v>81.106795948699997</v>
       </c>
       <c r="J67">
         <v>4.52914529281</v>
@@ -5625,8 +5885,12 @@
       <c r="Y67">
         <v>83.406832734999995</v>
       </c>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z67">
+        <f t="shared" ref="Z67:Z102" si="1">I67+100</f>
+        <v>181.10679594869998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>16.5</v>
       </c>
@@ -5652,7 +5916,7 @@
         <v>34</v>
       </c>
       <c r="I68">
-        <v>-19.767014738699999</v>
+        <v>80.232985261300001</v>
       </c>
       <c r="J68">
         <v>4.3526880281700002</v>
@@ -5702,8 +5966,12 @@
       <c r="Y68">
         <v>84.756216673400004</v>
       </c>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z68">
+        <f t="shared" si="1"/>
+        <v>180.2329852613</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>16.75</v>
       </c>
@@ -5729,7 +5997,7 @@
         <v>33</v>
       </c>
       <c r="I69">
-        <v>-20.681239170400001</v>
+        <v>79.318760829599995</v>
       </c>
       <c r="J69">
         <v>4.1850536267600003</v>
@@ -5779,8 +6047,12 @@
       <c r="Y69">
         <v>86.0159219409</v>
       </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z69">
+        <f t="shared" si="1"/>
+        <v>179.3187608296</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>17</v>
       </c>
@@ -5806,7 +6078,7 @@
         <v>32</v>
       </c>
       <c r="I70">
-        <v>-21.637746482000001</v>
+        <v>78.362253518000003</v>
       </c>
       <c r="J70">
         <v>4.0258009454200003</v>
@@ -5856,8 +6128,12 @@
       <c r="Y70">
         <v>87.188703973499997</v>
       </c>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z70">
+        <f t="shared" si="1"/>
+        <v>178.36225351799999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>17.25</v>
       </c>
@@ -5883,7 +6159,7 @@
         <v>31</v>
       </c>
       <c r="I71">
-        <v>-22.638492256799999</v>
+        <v>77.361507743200008</v>
       </c>
       <c r="J71">
         <v>3.87451089815</v>
@@ -5933,8 +6209,12 @@
       <c r="Y71">
         <v>88.277779262799996</v>
       </c>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z71">
+        <f t="shared" si="1"/>
+        <v>177.36150774320001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>17.5</v>
       </c>
@@ -5960,7 +6240,7 @@
         <v>30</v>
       </c>
       <c r="I72">
-        <v>-23.685522523700001</v>
+        <v>76.314477476299999</v>
       </c>
       <c r="J72">
         <v>3.7307853532399999</v>
@@ -6010,8 +6290,12 @@
       <c r="Y72">
         <v>89.286720587199994</v>
       </c>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z72">
+        <f t="shared" si="1"/>
+        <v>176.3144774763</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>17.75</v>
       </c>
@@ -6037,7 +6321,7 @@
         <v>29</v>
       </c>
       <c r="I73">
-        <v>-24.7809779404</v>
+        <v>75.219022059600007</v>
       </c>
       <c r="J73">
         <v>3.59424608558</v>
@@ -6087,8 +6371,12 @@
       <c r="Y73">
         <v>90.219360333099999</v>
       </c>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z73">
+        <f t="shared" si="1"/>
+        <v>175.21902205960001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>18</v>
       </c>
@@ -6114,7 +6402,7 @@
         <v>28</v>
       </c>
       <c r="I74">
-        <v>-25.927098170200001</v>
+        <v>74.072901829800003</v>
       </c>
       <c r="J74">
         <v>3.4645337813000001</v>
@@ -6164,8 +6452,12 @@
       <c r="Y74">
         <v>91.079703311100005</v>
       </c>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z74">
+        <f t="shared" si="1"/>
+        <v>174.0729018298</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>18.25</v>
       </c>
@@ -6191,7 +6483,7 @@
         <v>27</v>
       </c>
       <c r="I75">
-        <v>-27.1262264605</v>
+        <v>72.873773539500007</v>
       </c>
       <c r="J75">
         <v>3.3413070922300001</v>
@@ -6241,8 +6533,12 @@
       <c r="Y75">
         <v>91.871849837599996</v>
       </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z75">
+        <f t="shared" si="1"/>
+        <v>172.87377353950001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>18.5</v>
       </c>
@@ -6268,7 +6564,7 @@
         <v>26</v>
       </c>
       <c r="I76">
-        <v>-28.3808144343</v>
+        <v>71.619185565700008</v>
       </c>
       <c r="J76">
         <v>3.2242417376199999</v>
@@ -6318,8 +6614,12 @@
       <c r="Y76">
         <v>92.599929324000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z76">
+        <f t="shared" si="1"/>
+        <v>171.61918556570001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>18.75</v>
       </c>
@@ -6345,7 +6645,7 @@
         <v>25</v>
       </c>
       <c r="I77">
-        <v>-29.693427101899999</v>
+        <v>70.306572898100001</v>
       </c>
       <c r="J77">
         <v>3.1130296507400002</v>
@@ -6395,8 +6695,12 @@
       <c r="Y77">
         <v>93.268044195000002</v>
       </c>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z77">
+        <f t="shared" si="1"/>
+        <v>170.3065728981</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>19</v>
       </c>
@@ -6422,7 +6726,7 @@
         <v>24</v>
       </c>
       <c r="I78">
-        <v>-31.066748105399999</v>
+        <v>68.933251894600005</v>
       </c>
       <c r="J78">
         <v>3.0073781681999998</v>
@@ -6472,8 +6776,12 @@
       <c r="Y78">
         <v>93.8802236378</v>
       </c>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z78">
+        <f t="shared" si="1"/>
+        <v>168.93325189460001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>19.25</v>
       </c>
@@ -6499,7 +6807,7 @@
         <v>23</v>
       </c>
       <c r="I79">
-        <v>-32.503585205199997</v>
+        <v>67.496414794800003</v>
       </c>
       <c r="J79">
         <v>2.9070092597900001</v>
@@ -6549,8 +6857,12 @@
       <c r="Y79">
         <v>94.440386461900005</v>
       </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z79">
+        <f t="shared" si="1"/>
+        <v>167.49641479479999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>19.5</v>
       </c>
@@ -6576,7 +6888,7 @@
         <v>22</v>
       </c>
       <c r="I80">
-        <v>-34.006876020999997</v>
+        <v>65.993123979000003</v>
       </c>
       <c r="J80">
         <v>2.8116587968000002</v>
@@ -6626,8 +6938,12 @@
       <c r="Y80">
         <v>94.952312211800006</v>
       </c>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z80">
+        <f t="shared" si="1"/>
+        <v>165.99312397900002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>19.75</v>
       </c>
@@ -6653,7 +6969,7 @@
         <v>21</v>
       </c>
       <c r="I81">
-        <v>-35.579694037000003</v>
+        <v>64.420305963000004</v>
       </c>
       <c r="J81">
         <v>2.7210758569600002</v>
@@ -6703,8 +7019,12 @@
       <c r="Y81">
         <v>95.419619597899995</v>
       </c>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z81">
+        <f t="shared" si="1"/>
+        <v>164.420305963</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>20</v>
       </c>
@@ -6730,7 +7050,7 @@
         <v>20</v>
       </c>
       <c r="I82">
-        <v>-37.225254886199998</v>
+        <v>62.774745113800002</v>
       </c>
       <c r="J82">
         <v>2.6350220641200002</v>
@@ -6780,8 +7100,12 @@
       <c r="Y82">
         <v>95.845751299599996</v>
       </c>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z82">
+        <f t="shared" si="1"/>
+        <v>162.77474511380001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>20.25</v>
       </c>
@@ -6807,7 +7131,7 @@
         <v>19</v>
       </c>
       <c r="I83">
-        <v>-38.946922924699997</v>
+        <v>61.053077075300003</v>
       </c>
       <c r="J83">
         <v>2.5532709609099999</v>
@@ -6857,8 +7181,12 @@
       <c r="Y83">
         <v>96.2339642102</v>
       </c>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z83">
+        <f t="shared" si="1"/>
+        <v>161.0530770753</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>20.5</v>
       </c>
@@ -6884,7 +7212,7 @@
         <v>18</v>
       </c>
       <c r="I84">
-        <v>-40.748218109900002</v>
+        <v>59.251781890099998</v>
       </c>
       <c r="J84">
         <v>2.4756074128700001</v>
@@ -6934,8 +7262,12 @@
       <c r="Y84">
         <v>96.587324249800005</v>
       </c>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z84">
+        <f t="shared" si="1"/>
+        <v>159.25178189010001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>20.75</v>
       </c>
@@ -6961,7 +7293,7 @@
         <v>17</v>
       </c>
       <c r="I85">
-        <v>-42.632823197500002</v>
+        <v>57.367176802499998</v>
       </c>
       <c r="J85">
         <v>2.4018270422199999</v>
@@ -7011,8 +7343,12 @@
       <c r="Y85">
         <v>96.908704938499994</v>
       </c>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z85">
+        <f t="shared" si="1"/>
+        <v>157.36717680250001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>21</v>
       </c>
@@ -7038,7 +7374,7 @@
         <v>16</v>
       </c>
       <c r="I86">
-        <v>-44.6045912704</v>
+        <v>55.3954087296</v>
       </c>
       <c r="J86">
         <v>2.3317356901099999</v>
@@ -7088,8 +7424,12 @@
       <c r="Y86">
         <v>97.200789004499995</v>
       </c>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z86">
+        <f t="shared" si="1"/>
+        <v>155.39540872960001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>21.25</v>
       </c>
@@ -7115,7 +7455,7 @@
         <v>15</v>
       </c>
       <c r="I87">
-        <v>-46.667553616600003</v>
+        <v>53.332446383399997</v>
       </c>
       <c r="J87">
         <v>2.2651489056099998</v>
@@ -7165,8 +7505,12 @@
       <c r="Y87">
         <v>97.466072383899998</v>
       </c>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z87">
+        <f t="shared" si="1"/>
+        <v>153.3324463834</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>21.5</v>
       </c>
@@ -7192,7 +7536,7 @@
         <v>14</v>
       </c>
       <c r="I88">
-        <v>-48.825927971399999</v>
+        <v>51.174072028600001</v>
       </c>
       <c r="J88">
         <v>2.2018914603200002</v>
@@ -7242,8 +7586,12 @@
       <c r="Y88">
         <v>97.706870057000003</v>
       </c>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z88">
+        <f t="shared" si="1"/>
+        <v>151.17407202859999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>21.75</v>
       </c>
@@ -7269,7 +7617,7 @@
         <v>13</v>
       </c>
       <c r="I89">
-        <v>-51.084127140100001</v>
+        <v>48.915872859899999</v>
       </c>
       <c r="J89">
         <v>2.14179688731</v>
@@ -7319,8 +7667,12 @@
       <c r="Y89">
         <v>97.925323242700003</v>
       </c>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z89">
+        <f t="shared" si="1"/>
+        <v>148.91587285989999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>22</v>
       </c>
@@ -7346,7 +7698,7 @@
         <v>12</v>
       </c>
       <c r="I90">
-        <v>-53.446768020299999</v>
+        <v>46.553231979700001</v>
       </c>
       <c r="J90">
         <v>2.0847070429399999</v>
@@ -7396,8 +7748,12 @@
       <c r="Y90">
         <v>98.123407549999996</v>
       </c>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z90">
+        <f t="shared" si="1"/>
+        <v>146.5532319797</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>22.25</v>
       </c>
@@ -7423,7 +7779,7 @@
         <v>11</v>
       </c>
       <c r="I91">
-        <v>-55.918681041299998</v>
+        <v>44.081318958700002</v>
       </c>
       <c r="J91">
         <v>2.0304716907999998</v>
@@ -7473,8 +7829,12 @@
       <c r="Y91">
         <v>98.302941754599999</v>
       </c>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z91">
+        <f t="shared" si="1"/>
+        <v>144.0813189587</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>22.5</v>
       </c>
@@ -7500,7 +7860,7 @@
         <v>10</v>
       </c>
       <c r="I92">
-        <v>-58.504920039399998</v>
+        <v>41.495079960600002</v>
       </c>
       <c r="J92">
         <v>1.9789481062600001</v>
@@ -7550,8 +7910,12 @@
       <c r="Y92">
         <v>98.465596927000007</v>
       </c>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z92">
+        <f t="shared" si="1"/>
+        <v>141.49507996060001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>22.75</v>
       </c>
@@ -7577,7 +7941,7 @@
         <v>9</v>
       </c>
       <c r="I93">
-        <v>-61.210772591199998</v>
+        <v>38.789227408800002</v>
       </c>
       <c r="J93">
         <v>1.93000070094</v>
@@ -7627,8 +7991,12 @@
       <c r="Y93">
         <v>98.612905693599998</v>
       </c>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z93">
+        <f t="shared" si="1"/>
+        <v>138.7892274088</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>23</v>
       </c>
@@ -7654,7 +8022,7 @@
         <v>8</v>
       </c>
       <c r="I94">
-        <v>-64.041770823600004</v>
+        <v>35.958229176399996</v>
       </c>
       <c r="J94">
         <v>1.8835006659</v>
@@ -7704,8 +8072,12 @@
       <c r="Y94">
         <v>98.746271458699994</v>
       </c>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z94">
+        <f t="shared" si="1"/>
+        <v>135.95822917639998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>23.25</v>
       </c>
@@ -7731,7 +8103,7 @@
         <v>7</v>
       </c>
       <c r="I95">
-        <v>-67.003702724199997</v>
+        <v>32.996297275800003</v>
       </c>
       <c r="J95">
         <v>1.8393256326</v>
@@ -7781,8 +8153,12 @@
       <c r="Y95">
         <v>98.866977452100002</v>
       </c>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z95">
+        <f t="shared" si="1"/>
+        <v>132.9962972758</v>
+      </c>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>23.5</v>
       </c>
@@ -7808,7 +8184,7 @@
         <v>6</v>
       </c>
       <c r="I96">
-        <v>-70.102623975200004</v>
+        <v>29.897376024799996</v>
       </c>
       <c r="J96">
         <v>1.7973593509700001</v>
@@ -7858,8 +8234,12 @@
       <c r="Y96">
         <v>98.976195503900001</v>
       </c>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z96">
+        <f t="shared" si="1"/>
+        <v>129.8973760248</v>
+      </c>
+    </row>
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>23.75</v>
       </c>
@@ -7885,7 +8265,7 @@
         <v>5</v>
       </c>
       <c r="I97">
-        <v>-73.344870334000007</v>
+        <v>26.655129665999993</v>
       </c>
       <c r="J97">
         <v>1.7574913834200001</v>
@@ -7935,8 +8315,12 @@
       <c r="Y97">
         <v>99.074994470999997</v>
       </c>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z97">
+        <f t="shared" si="1"/>
+        <v>126.65512966599999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>24</v>
       </c>
@@ -7962,7 +8346,7 @@
         <v>4</v>
       </c>
       <c r="I98">
-        <v>-76.737070587000005</v>
+        <v>23.262929412999995</v>
       </c>
       <c r="J98">
         <v>1.7196168142499999</v>
@@ -8012,8 +8396,12 @@
       <c r="Y98">
         <v>99.164348265699999</v>
       </c>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z98">
+        <f t="shared" si="1"/>
+        <v>123.26292941299999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>24.25</v>
       </c>
@@ -8039,7 +8427,7 @@
         <v>3</v>
       </c>
       <c r="I99">
-        <v>-80.286160101600004</v>
+        <v>19.713839898399996</v>
       </c>
       <c r="J99">
         <v>1.6836359735399999</v>
@@ -8089,8 +8477,12 @@
       <c r="Y99">
         <v>99.245143453899999</v>
       </c>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z99">
+        <f t="shared" si="1"/>
+        <v>119.7138398984</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>24.5</v>
       </c>
@@ -8116,7 +8508,7 @@
         <v>2</v>
       </c>
       <c r="I100">
-        <v>-83.999395006300006</v>
+        <v>16.000604993699994</v>
       </c>
       <c r="J100">
         <v>1.64945417486</v>
@@ -8166,8 +8558,12 @@
       <c r="Y100">
         <v>99.3181864039</v>
       </c>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z100">
+        <f t="shared" si="1"/>
+        <v>116.00060499369999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>24.75</v>
       </c>
@@ -8193,7 +8589,7 @@
         <v>1</v>
       </c>
       <c r="I101">
-        <v>-87.884367025399996</v>
+        <v>12.115632974600004</v>
       </c>
       <c r="J101">
         <v>1.6169814661199999</v>
@@ -8243,8 +8639,12 @@
       <c r="Y101">
         <v>99.384209981500007</v>
       </c>
-    </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z101">
+        <f t="shared" si="1"/>
+        <v>112.1156329746</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>25</v>
       </c>
@@ -8270,7 +8670,7 @@
         <v>0</v>
       </c>
       <c r="I102">
-        <v>-91.949019000299998</v>
+        <v>8.0509809997000019</v>
       </c>
       <c r="J102">
         <v>1.58613239281</v>
@@ -8319,6 +8719,10 @@
       </c>
       <c r="Y102">
         <v>99.443879790899999</v>
+      </c>
+      <c r="Z102">
+        <f t="shared" si="1"/>
+        <v>108.0509809997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>